<commit_message>
Added comments and presentation
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wmuyoma16\Documents\GitHub\DataStructuresFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\The Real Folders\Documents\GitHub\DataStructuresFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -149,7 +149,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Patient Visit Time for Different Staff Arragements </a:t>
+              <a:t> Patient Visit Time for Different Staff Arrangements </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -251,11 +251,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="409184152"/>
-        <c:axId val="409158280"/>
+        <c:axId val="323522240"/>
+        <c:axId val="323523808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="409184152"/>
+        <c:axId val="323522240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -282,11 +282,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Diffrent</a:t>
+                  <a:t>Diffrerent</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Staff Arragements</a:t>
+                  <a:t> Staff Arrangements</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -359,7 +359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409158280"/>
+        <c:crossAx val="323523808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -367,7 +367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="409158280"/>
+        <c:axId val="323523808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,16 +446,13 @@
                   <a:buFontTx/>
                   <a:buNone/>
                   <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr>
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:sysClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -537,7 +534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409184152"/>
+        <c:crossAx val="323522240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -601,6 +598,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Visit Time for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Varying Rates of Arrival</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -660,7 +687,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -673,6 +700,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="34925" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet2!$A$7:$A$18</c:f>
@@ -773,11 +814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346506744"/>
-        <c:axId val="346505960"/>
+        <c:axId val="323521064"/>
+        <c:axId val="323521456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346506744"/>
+        <c:axId val="323521064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,12 +936,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346505960"/>
+        <c:crossAx val="323521456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="346505960"/>
+        <c:axId val="323521456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +1059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346506744"/>
+        <c:crossAx val="323521064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2502,7 +2543,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2630,7 +2671,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>